<commit_message>
feat: make a basic data structure
rememberer-bot
</commit_message>
<xml_diff>
--- a/описание_комнат_и_задач.xlsx
+++ b/описание_комнат_и_задач.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan\PyCharm\Rememberer-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{172A3192-7F4C-4662-AC78-F75C46F96DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962260F4-CF42-4C37-8594-325E46E2C9E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{62E945CA-B744-4C8F-A85E-82BFD8AFAAD8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>Текст задачи</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t>Список получателей</t>
+  </si>
+  <si>
+    <t>Поля юзера</t>
+  </si>
+  <si>
+    <t>telegram_ID</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>группа</t>
+  </si>
+  <si>
+    <t>роль в группе</t>
   </si>
 </sst>
 </file>
@@ -167,10 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -485,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B967A8D2-9898-4757-AF40-01AA5A0F4490}">
-  <dimension ref="B5:K23"/>
+  <dimension ref="B5:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,13 +531,13 @@
       <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -563,7 +577,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -583,7 +597,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
@@ -623,7 +637,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="1"/>
@@ -647,7 +661,7 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="1"/>
@@ -771,6 +785,40 @@
       </c>
       <c r="H23" s="1"/>
     </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>